<commit_message>
Changed the colorectal mutation definitions for KRAS & NRAS, so the codons agree with what the reports say.
</commit_message>
<xml_diff>
--- a/reportgen/assets/COLORECTAL_MUTATION_TABLE.xlsx
+++ b/reportgen/assets/COLORECTAL_MUTATION_TABLE.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeckabergstrom/repos/reportgen/reportgen/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="18560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="18560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
@@ -13,6 +18,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="177">
   <si>
     <t>BRAF</t>
   </si>
@@ -98,12 +106,6 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>12,13,61</t>
-  </si>
-  <si>
-    <t>12,13,60,61,117,146</t>
-  </si>
-  <si>
     <t>Adjusted PIK3CA, KRAS and NRAS hotspots after findings in Chang et al (Identifying recurrent mutations in cancer reveals widespread lineage diversity and mutational specificity). More stringence on PTEN and PIK3R1 after meeting with group. Added focal amp of IGF2 as (preliminary, pending technical sensitivity) addition to class B.</t>
   </si>
   <si>
@@ -555,6 +557,9 @@
   </si>
   <si>
     <t>p.Val600Glu</t>
+  </si>
+  <si>
+    <t>12,13,59,61,117,146</t>
   </si>
 </sst>
 </file>
@@ -1054,6 +1059,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1383,10 +1393,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -1398,12 +1408,12 @@
     <col min="9" max="9" width="99" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1412,13 +1422,13 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1432,14 +1442,14 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1453,14 +1463,14 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="F3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1474,281 +1484,276 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
       <c r="F4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="E8"/>
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E9"/>
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14"/>
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15"/>
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="E16"/>
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="E17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="E18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="E19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="E20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="E21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="E22"/>
       <c r="I22"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="E23"/>
       <c r="I23"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="E24"/>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="E25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="E26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="E27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="E28"/>
       <c r="I28"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="5"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="5"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="5"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="5"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="5"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="5"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="5"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="5"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="5"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="5"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="5"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="5"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="5"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="5"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="5"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="5"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="5"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="5"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="5"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="5"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="5"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="5"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="5"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="5"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="5"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="5"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="5"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="5"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1760,12 +1765,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1773,7 +1778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1781,29 +1786,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1815,7 +1815,7 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
@@ -1825,635 +1825,630 @@
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
         <v>164</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>166</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>103</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>104</v>
       </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>106</v>
-      </c>
       <c r="F7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>108</v>
       </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>110</v>
-      </c>
       <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
         <v>115</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>116</v>
       </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
-      </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T13" s="9"/>
       <c r="Z13" s="9"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
         <v>119</v>
       </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
         <v>120</v>
       </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="B15" t="s">
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>121</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>122</v>
       </c>
-      <c r="F15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="B16" t="s">
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>123</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>124</v>
       </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" t="s">
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>125</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>126</v>
       </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
+      <c r="F18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
         <v>127</v>
       </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
         <v>128</v>
       </c>
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>129</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>130</v>
       </c>
-      <c r="F19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" t="s">
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>131</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>132</v>
       </c>
-      <c r="F20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" t="s">
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>133</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>134</v>
       </c>
-      <c r="F21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>135</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>136</v>
       </c>
-      <c r="F22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" t="s">
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>137</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>138</v>
       </c>
-      <c r="F23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" t="s">
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>68</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>139</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>69</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>140</v>
       </c>
-      <c r="F24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" t="s">
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>141</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>71</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>142</v>
       </c>
-      <c r="F25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" t="s">
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>143</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>73</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>144</v>
       </c>
-      <c r="F26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" t="s">
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>145</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>75</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>146</v>
       </c>
-      <c r="F27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" t="s">
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>76</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>147</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>77</v>
       </c>
-      <c r="E28" t="s">
-        <v>148</v>
-      </c>
-      <c r="F28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" t="s">
+      <c r="C30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
-        <v>149</v>
-      </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>150</v>
       </c>
-      <c r="F29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" t="s">
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>79</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>151</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>80</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>152</v>
       </c>
-      <c r="F30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" t="s">
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>153</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>82</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E32" t="s">
         <v>154</v>
       </c>
-      <c r="F31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" t="s">
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>83</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>155</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>84</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>156</v>
       </c>
-      <c r="F32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
+      <c r="F33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>85</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="s">
         <v>157</v>
       </c>
-      <c r="D33" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="F34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
         <v>158</v>
       </c>
-      <c r="F33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>88</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>159</v>
       </c>
-      <c r="F34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>89</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>160</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>90</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>161</v>
       </c>
-      <c r="F35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" t="s">
-        <v>162</v>
-      </c>
-      <c r="D36" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" t="s">
-        <v>163</v>
-      </c>
       <c r="F36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>